<commit_message>
Rewrite ExctractToExcel mathod in ExtractExcelFromSQLite class
</commit_message>
<xml_diff>
--- a/ExcelFromSQLite/Products.xlsx
+++ b/ExcelFromSQLite/Products.xlsx
@@ -5,26 +5,13 @@
     <workbookView/>
   </bookViews>
   <sheets>
-    <sheet name="Products" sheetId="1" r:id="R8d5fdfd156fe45c7"/>
+    <sheet name="Products" sheetId="1" r:id="R2bf170be2a3a4f0b"/>
   </sheets>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>ProductId</t>
-  </si>
-  <si>
-    <t>SoldPieces</t>
-  </si>
-  <si>
-    <t>StartData</t>
-  </si>
-  <si>
-    <t>EndDate</t>
-  </si>
-</sst>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="0" uniqueCount="0"/>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -68,27 +55,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
-  <sheetData>
-    <row r="1">
-      <c r="A1" s="0" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="0" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="0" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="0" t="s">
-        <v>3</v>
-      </c>
-    </row>
-  </sheetData>
+  <sheetData/>
   <headerFooter/>
 </worksheet>
 </file>
</xml_diff>